<commit_message>
Requirements & Parts List Update
Updated requirements for SW debug mode
Updated Electrical Parts List - 12" ribbon to 18" ribbon
</commit_message>
<xml_diff>
--- a/Electrical/Schematic/Electrical Parts List.xlsx
+++ b/Electrical/Schematic/Electrical Parts List.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="112">
   <si>
     <t>Description</t>
   </si>
@@ -114,12 +112,6 @@
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>1M-1010-016-3365-012.0-00-AB-00-0</t>
-  </si>
-  <si>
-    <t>3M 12" - 16 Pin Ribbon Cable</t>
-  </si>
-  <si>
     <t>22-01-2035</t>
   </si>
   <si>
@@ -217,13 +209,154 @@
   </si>
   <si>
     <t># Connectors</t>
+  </si>
+  <si>
+    <t>3M 18" - 16 Pin Ribbon Cable</t>
+  </si>
+  <si>
+    <t>1M-1010-016-3365-018.0-00-AB-00-0</t>
+  </si>
+  <si>
+    <t>Mouser Part #</t>
+  </si>
+  <si>
+    <t>538-22-23-2101</t>
+  </si>
+  <si>
+    <t>538-22-01-2105</t>
+  </si>
+  <si>
+    <t>538-22-23-2071</t>
+  </si>
+  <si>
+    <t>538-22-01-2075</t>
+  </si>
+  <si>
+    <t>538-22-23-2031</t>
+  </si>
+  <si>
+    <t>538-22-01-2035</t>
+  </si>
+  <si>
+    <t>71-CPF15R0000BEE14</t>
+  </si>
+  <si>
+    <t>279-YR1B2K0CC</t>
+  </si>
+  <si>
+    <t>279-YR1B100RCC</t>
+  </si>
+  <si>
+    <t>584-AD623ANZ</t>
+  </si>
+  <si>
+    <t>998-MIC2920A-4.8WT</t>
+  </si>
+  <si>
+    <t>538-22-23-2021</t>
+  </si>
+  <si>
+    <t>538-22-01-2025</t>
+  </si>
+  <si>
+    <t>538-22-23-2041</t>
+  </si>
+  <si>
+    <t>538-22-01-2045</t>
+  </si>
+  <si>
+    <t>538-22-23-2051</t>
+  </si>
+  <si>
+    <t>538-22-01-2055</t>
+  </si>
+  <si>
+    <t>517-1M-1010-016-18</t>
+  </si>
+  <si>
+    <t>571-5103309-3</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-23-2101/?qs=%2fha2pyFadugjgDurvcIWB8s4U7rRBv7%2fXzPPvZh4JX4%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-01-2105/?qs=sGAEpiMZZMtVoztFdqDXO3DRJJT96OZO</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-23-2071/?qs=%2fha2pyFadui05csbord1TL%252bFEJkHeXS5tqBPXMg0IfU%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-01-2075/?qs=%2fha2pyFadujIEQkzoGlziyCT2TtB1sfc1hh%252bXZeGnjk%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-23-2031/?qs=%2fha2pyFadui05csbord1TDqxqV9YYod2gbgFgLhsgQs%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-01-2035/?qs=%2fha2pyFadujIEQkzoGlzi6OdgxxLl5ZwtIU0IZrEPkY%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay/CPF15R0000BEE14/?qs=%2fha2pyFaduiaZsVQamaA2J%2f3iz%2f6Bk8JRgloa4Nu6fiy5xTYjd%252bk1g%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TE-Connectivity/YR1B2K0CC/?qs=%2fha2pyFadugZtfbfcI14SzXntEB%2fS%252bvN37mPtL%2fEKUU%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TE-Connectivity/YR1B100RCC/?qs=%2fha2pyFadujfkjl%2fw2CT8wH4dU44PFFTyZyFDkshbTA0fGbLwSa2EA%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Analog-Devices-Inc/AD623ANZ/?qs=%2fha2pyFaduhdIfUTQsr%2fvczIzdxo3lXhsoU0t5GYykc%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Micrel/MIC2920A-48WT/?qs=sGAEpiMZZMv7pcWEpiAU7BWpw0WMjQJh</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-23-2021/?qs=%2fha2pyFadui05csbord1TERiu2NYJxjoklgO5wLkQY4%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-01-2025/?qs=%2fha2pyFadujIEQkzoGlzi18osD4%2fb1HiF9yjQ%252bQVUaw%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-23-2041/?qs=%2fha2pyFadui05csbord1TMsF5snYzfCUIYoKbwTHl0Q%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-01-2045/?qs=%2fha2pyFadujIEQkzoGlzi559yoLnPoJw%252bGSnVTNWap0%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-23-2051/?qs=%2fha2pyFadui05csbord1TAl15AOjOR7%252bevVIf1oesso%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/22-01-2055/?qs=sGAEpiMZZMtVoztFdqDXO75tY90O5CVx</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/3M/1M-1010-016-3365-0180-00-AB-00-0/?qs=%2fha2pyFadugupELTcRboixIeeCaNTh7GJwFkE%2f5%2fCe85iYZ%252b5u%252bS8F4vQnUcNp8FhfyL817limQ%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TE-Connectivity/5103309-3/?qs=sGAEpiMZZMs%252bGHln7q6pm%252bE9wskmeR%2fSEd6EQezELx0%3d</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Change length/part for ribbon cable from 12" to 18"</t>
+  </si>
+  <si>
+    <t>Added Mouser part numbers and Links</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +376,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +412,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -497,10 +658,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -517,17 +679,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -559,8 +712,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -860,118 +1034,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC26"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16383" width="9.140625" style="7"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="195.85546875" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="I1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20">
+      <c r="G2" s="17">
         <v>10</v>
       </c>
-      <c r="G2" s="23">
+      <c r="H2" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10" t="s">
+      <c r="I2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30"/>
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21">
+      <c r="G3" s="18">
         <v>10</v>
       </c>
-      <c r="G3" s="24">
+      <c r="H3" s="21">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="I3" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="20">
+      <c r="G4" s="17">
         <v>7</v>
       </c>
-      <c r="G4" s="23">
+      <c r="H4" s="20">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="I4" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -980,233 +1193,332 @@
         <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="6">
         <v>7</v>
       </c>
-      <c r="G5" s="25">
+      <c r="H5" s="22">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="I5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="22">
+        <v>8</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+      <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="C7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="18">
         <v>3</v>
       </c>
-      <c r="F6" s="6">
-        <v>3</v>
-      </c>
-      <c r="G6" s="25">
+      <c r="H7" s="21">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="21">
-        <v>3</v>
-      </c>
-      <c r="G7" s="24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="23">
+      <c r="I7" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="20">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="I8" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="25">
+        <v>50</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="22">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="I9" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="22">
+        <v>9</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="22">
+        <v>9</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="24">
+      <c r="D12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="21">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="13" t="s">
+      <c r="I12" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="20">
+      <c r="G13" s="17">
         <v>2</v>
       </c>
-      <c r="G13" s="23">
+      <c r="H13" s="20">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="I13" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="21">
+      <c r="G14" s="18">
         <v>2</v>
       </c>
-      <c r="G14" s="24">
+      <c r="H14" s="21">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="I14" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="20">
+      <c r="G15" s="17">
         <v>2</v>
       </c>
-      <c r="G15" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="H15" s="20">
+        <v>1</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1216,18 +1528,27 @@
       <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="6">
+      <c r="G16" s="6">
         <v>2</v>
       </c>
-      <c r="G16" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="H16" s="22">
+        <v>1</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="29"/>
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1237,62 +1558,89 @@
       <c r="D17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="6">
+      <c r="G17" s="6">
         <v>2</v>
       </c>
-      <c r="G17" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10" t="s">
+      <c r="H17" s="22">
+        <v>1</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="21">
+      <c r="G18" s="18">
         <v>2</v>
       </c>
-      <c r="G18" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="13" t="s">
+      <c r="H18" s="21">
+        <v>1</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="20">
+      <c r="G19" s="17">
         <v>2</v>
       </c>
-      <c r="G19" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="H19" s="20">
+        <v>1</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1302,18 +1650,27 @@
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="6">
+      <c r="G20" s="6">
         <v>2</v>
       </c>
-      <c r="G20" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="H20" s="22">
+        <v>1</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1324,17 +1681,26 @@
         <v>23</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="6">
+      <c r="G21" s="6">
         <v>4</v>
       </c>
-      <c r="G21" s="25">
+      <c r="H21" s="22">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="I21" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1345,17 +1711,26 @@
         <v>22</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <v>4</v>
       </c>
-      <c r="G22" s="25">
+      <c r="H22" s="22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="I22" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1366,17 +1741,26 @@
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="6">
+      <c r="G23" s="6">
         <v>5</v>
       </c>
-      <c r="G23" s="25">
+      <c r="H23" s="22">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="I23" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1387,94 +1771,143 @@
         <v>8</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G24" s="6">
         <v>5</v>
       </c>
-      <c r="G24" s="25">
+      <c r="H24" s="22">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="I24" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
+      <c r="C25" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10" t="s">
+      <c r="H25" s="22">
+        <v>1</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="30"/>
+      <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="G26" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="24">
-        <v>1</v>
+      <c r="H26" s="21">
+        <v>1</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
+        <v>42316</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>42316</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A19:A26"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A19:A26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D26" r:id="rId1" display="http://www.mouser.com/ProductDetail/TE-Connectivity/5103309-3/?qs=sGAEpiMZZMs%252bGHln7q6pm%252bE9wskmeR%2fSEd6EQezELx0%3d"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="J4" r:id="rId4"/>
+    <hyperlink ref="J5" r:id="rId5"/>
+    <hyperlink ref="J6" r:id="rId6"/>
+    <hyperlink ref="J7" r:id="rId7"/>
+    <hyperlink ref="J8" r:id="rId8"/>
+    <hyperlink ref="J9" r:id="rId9"/>
+    <hyperlink ref="J10" r:id="rId10"/>
+    <hyperlink ref="J11" r:id="rId11"/>
+    <hyperlink ref="J12" r:id="rId12"/>
+    <hyperlink ref="J13" r:id="rId13"/>
+    <hyperlink ref="J14" r:id="rId14"/>
+    <hyperlink ref="J15" r:id="rId15"/>
+    <hyperlink ref="J16" r:id="rId16"/>
+    <hyperlink ref="J17" r:id="rId17"/>
+    <hyperlink ref="J18" r:id="rId18"/>
+    <hyperlink ref="J19" r:id="rId19"/>
+    <hyperlink ref="J20" r:id="rId20"/>
+    <hyperlink ref="J21" r:id="rId21"/>
+    <hyperlink ref="J22" r:id="rId22"/>
+    <hyperlink ref="J23" r:id="rId23"/>
+    <hyperlink ref="J24" r:id="rId24"/>
+    <hyperlink ref="J26" r:id="rId25"/>
+    <hyperlink ref="J25" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MOV addition to circuit
MOV added to circuit to suppress voltage spikes caused by switching off
the inductive load of the pumps.
</commit_message>
<xml_diff>
--- a/Electrical/Schematic/Electrical Parts List.xlsx
+++ b/Electrical/Schematic/Electrical Parts List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="118">
   <si>
     <t>Description</t>
   </si>
@@ -350,13 +350,34 @@
   </si>
   <si>
     <t>Added Mouser part numbers and Links</t>
+  </si>
+  <si>
+    <t>Varistors (MOV)</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>Varistors 130volts 2500A</t>
+  </si>
+  <si>
+    <t>B72210S0131K101</t>
+  </si>
+  <si>
+    <t>871-B72210S131K101</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/EPCOS-TDK/B72210S0131K101?qs=%2fha2pyFaduhnNYlvdOReOSOGbAqbgH4hoymzM8rrfzip5Zb74YmzSA%3d%3d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,8 +413,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +453,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -662,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -721,6 +756,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -730,8 +767,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1034,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1135,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1120,7 +1167,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
@@ -1150,7 +1197,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1182,7 +1229,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1212,7 +1259,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1242,7 +1289,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1319,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="30" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1304,7 +1351,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>47</v>
       </c>
@@ -1334,7 +1381,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1364,7 +1411,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1394,7 +1441,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
@@ -1424,7 +1471,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1456,7 +1503,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1486,7 +1533,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="30" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -1518,7 +1565,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1548,7 +1595,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1578,7 +1625,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
@@ -1608,7 +1655,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="30" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -1640,7 +1687,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1670,7 +1717,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1700,7 +1747,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1730,7 +1777,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1760,7 +1807,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1790,7 +1837,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1820,7 +1867,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1850,12 +1897,12 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="29" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="31">
+      <c r="A30" s="28">
         <v>42316</v>
       </c>
       <c r="B30" t="s">
@@ -1863,11 +1910,73 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="31">
+      <c r="A31" s="28">
         <v>42316</v>
       </c>
       <c r="B31" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="34"/>
+      <c r="B34" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="36">
+        <v>2</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2</v>
+      </c>
+      <c r="J34" s="37">
+        <f t="shared" ref="J34" si="0">H34+I34</f>
+        <v>4</v>
+      </c>
+      <c r="K34" s="38">
+        <v>0.54</v>
+      </c>
+      <c r="L34" s="38">
+        <f t="shared" ref="L34" si="1">J34*K34</f>
+        <v>2.16</v>
+      </c>
+      <c r="M34" s="38">
+        <f t="shared" ref="M34" si="2">ROUND(L34*6.5/100,2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N34" s="38">
+        <v>0</v>
+      </c>
+      <c r="O34" s="38">
+        <f t="shared" ref="O34" si="3">L34+M34+N34</f>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="P34" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q34" s="27" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1906,8 +2015,9 @@
     <hyperlink ref="J24" r:id="rId24"/>
     <hyperlink ref="J26" r:id="rId25"/>
     <hyperlink ref="J25" r:id="rId26"/>
+    <hyperlink ref="Q34" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>